<commit_message>
Simplified config sheet (v0.8.0)
* Allows the user to generate a minimally configured system based on a
  simplified configuration sheet.
* Overhaul of code that generates reports on population evolution +
  exporting those reports to Excel.
* Flux reports can be requested for a combination of transition (type)
  and source/target state.
* Allows retrieval of previously run simulation for further
  investigation.
</commit_message>
<xml_diff>
--- a/catalogueTest.xlsx
+++ b/catalogueTest.xlsx
@@ -5,18 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Attributes" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="States" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Transitions" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="State Map" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Recruitment" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Retirement" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Output plots" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Misc" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Snapshot" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="State Map" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Recruitment" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Retirement" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Output plots (trans)" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Output plots" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Misc" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -76,7 +78,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author> </author>
@@ -147,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="152">
   <si>
     <t xml:space="preserve">General simulation parameters</t>
   </si>
@@ -344,24 +346,63 @@
     <t xml:space="preserve">age</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cross-Promotion B to A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promotion A Master</t>
+  </si>
+  <si>
     <t xml:space="preserve">NO</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;=</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cross-Promotion B to A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Promotion A Master</t>
-  </si>
-  <si>
     <t xml:space="preserve">IS</t>
   </si>
   <si>
     <t xml:space="preserve">Promotion B master</t>
   </si>
   <si>
+    <t xml:space="preserve">Snapshot parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upload initial population?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snapshot file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testSnapshot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID column number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tenure info column number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is recruitment date?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age info column number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is birth date?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max columns to import</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># columns to import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Col nrs to import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute</t>
+  </si>
+  <si>
     <t xml:space="preserve">Plot of State Network</t>
   </si>
   <si>
@@ -462,6 +503,51 @@
   </si>
   <si>
     <t xml:space="preserve">satisfied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output graphs (transitions)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show plots?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate Excel?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excel filename</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testFluxReport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max flux plots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flux plots to show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source/Target?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transition name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time resolution (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">retired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resigned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fired</t>
   </si>
   <si>
     <t xml:space="preserve">Output graphs</t>
@@ -681,7 +767,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -774,6 +860,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -792,7 +882,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -820,6 +910,21 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -895,7 +1000,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -955,7 +1060,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -963,7 +1068,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1008,6 +1113,346 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="18"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="D3" s="3" t="n">
+        <f aca="false">MATCH(1,INDEX(ISBLANK(D6:$AMJ6),0,0),0)-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <dataValidations count="4">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 D6:E6" type="decimal">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B12 D12:E12" type="list">
+      <formula1>INDEX(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2),SMALL(IF(ISTEXT(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2)),ROW(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2))-ROW(Attributes!$A$6),""),ROW(INDIRECT("1:"&amp;Attributes!$B$4))))</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5 B7:B10 D7:E10 B13:B16 D13:E16" type="list">
+      <formula1>Misc!$B$1:$B$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:E5" type="list">
+      <formula1>OFFSET(States!$A$7,0,0,States!$B$4)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="20.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="3" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="n">
+        <f aca="true">INDIRECT(CONCATENATE("'",General!B3,".xlsx'#$General.B2"))</f>
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="str">
+        <f aca="false">IF(ISERR(A1),CONCATENATE("'[",General!B3,".xlsx]"),CONCATENATE("'",General!B3,".xlsx'#'"))</f>
+        <v>'simCatalogue.xlsx'#'</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="str">
+        <f aca="false">IF(ISERR(A1),"!",".")</f>
+        <v>.</v>
+      </c>
+      <c r="B3" s="0"/>
+      <c r="C3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <f aca="true">INDIRECT(CONCATENATE(A2,"General'",A3,"B1"))</f>
+        <v>0</v>
+      </c>
+      <c r="B4" s="0"/>
+      <c r="C4" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="str">
+        <f aca="false">CONCATENATE(A2,"General'",A3)</f>
+        <v>'simCatalogue.xlsx'#'General'.</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="str">
+        <f aca="false">CONCATENATE(A2,"Attributes'",A3)</f>
+        <v>'simCatalogue.xlsx'#'Attributes'.</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="str">
+        <f aca="false">CONCATENATE(A2,"States'",A3)</f>
+        <v>'simCatalogue.xlsx'#'States'.</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -1016,7 +1461,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1063,7 +1508,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="3" t="n">
-        <f aca="true">COUNTA(OFFSET(A7,0,0,B3*3))</f>
+        <f aca="true">COUNTA(OFFSET(A7,0,0,B3*3+1))</f>
         <v>4</v>
       </c>
       <c r="C4" s="3"/>
@@ -1336,7 +1781,7 @@
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1366,7 +1811,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="3" t="n">
-        <f aca="true">COUNTA(OFFSET(A7,0,0,B3))</f>
+        <f aca="true">MATCH(1,INDEX(ISBLANK(OFFSET(A7,0,0,B3+1)),0,0),0)-1</f>
         <v>6</v>
       </c>
     </row>
@@ -1506,8 +1951,12 @@
   </sheetPr>
   <dimension ref="A1:AME29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1897,9 +2346,11 @@
       <c r="M15" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="N15" s="15"/>
+      <c r="N15" s="15" t="n">
+        <v>1</v>
+      </c>
       <c r="O15" s="17" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="P15" s="3" t="n">
         <f aca="false">MATCH(1,INDEX(ISBLANK(Q15:$AMJ15),0,0),0)-1</f>
@@ -1921,7 +2372,7 @@
         <v>59</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T16" s="8" t="s">
         <v>24</v>
@@ -1932,7 +2383,7 @@
         <v>12</v>
       </c>
       <c r="I17" s="11" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1985,7 +2436,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>39</v>
@@ -2016,9 +2467,11 @@
       <c r="M19" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="N19" s="15"/>
+      <c r="N19" s="15" t="n">
+        <v>1</v>
+      </c>
       <c r="O19" s="17" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="P19" s="3" t="n">
         <f aca="false">MATCH(1,INDEX(ISBLANK(Q19:$AMJ19),0,0),0)-1</f>
@@ -2040,7 +2493,7 @@
         <v>59</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T20" s="8" t="s">
         <v>24</v>
@@ -2051,7 +2504,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="11" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,7 +2559,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>36</v>
@@ -2139,7 +2592,7 @@
       </c>
       <c r="N23" s="15"/>
       <c r="O23" s="17" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="P23" s="3" t="n">
         <f aca="false">MATCH(1,INDEX(ISBLANK(Q23:$AMJ23),0,0),0)-1</f>
@@ -2267,7 +2720,7 @@
       </c>
       <c r="N27" s="15"/>
       <c r="O27" s="17" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="P27" s="3" t="n">
         <f aca="false">MATCH(1,INDEX(ISBLANK(Q27:$AMJ27),0,0),0)-1</f>
@@ -2379,7 +2832,7 @@
       <formula>ISBLANK(N27)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="14">
+  <dataValidations count="15">
     <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -2420,7 +2873,7 @@
       <formula1>Misc!$C$1:$C$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K7 U7 K11 U11 T15 T19 K23 U23 K27 U27" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U7 K11 U11 T15 T19 K23 U23 K27 U27" type="list">
       <formula1>INDEX(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2),SMALL(IF(ISTEXT(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2)),ROW(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2))-ROW(Attributes!$A$6),""),ROW(INDIRECT("1:"&amp;Attributes!$B$4))))</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2434,6 +2887,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U8 U12 T16 T20 U24 U28" type="list">
       <formula1>OFFSET(INDIRECT(Misc!$A$6&amp;"F1"),MATCH(#ref!,OFFSET(INDIRECT(Misc!$A$6&amp;"A2"),0,0,INDIRECT(Misc!$A$5&amp;"B5"),1),0),0,1,OFFSET(INDIRECT(Misc!$A$6&amp;"E1"),MATCH(#ref!,OFFSET(INDIRECT(Misc!$A$6&amp;"A2"),0,0,INDIRECT(Misc!$A$5&amp;"B5"),1),0),0))</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K7" type="list">
+      <formula1>INDEX(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2),SMALL(IF(ISTEXT(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2)),ROW(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2))-ROW(Attributes!$A$6),""),ROW(INDIRECT("1:"&amp;Attributes!$B$4))))</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2452,118 +2909,169 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="18"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>65</v>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="2" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="8" t="n">
-        <v>1000</v>
+        <v>76</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="3" t="n">
-        <f aca="true">COUNTA(OFFSET(B9,0,0,B6))</f>
-        <v>6</v>
+        <v>77</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2" t="s">
-        <v>37</v>
+      <c r="A11" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="8" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="2" t="s">
-        <v>39</v>
+      <c r="A12" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="true">MATCH(1,INDEX(ISBLANK(OFFSET(A15,0,0,B11+1)),0,0),0)-1</f>
+        <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="2" t="s">
-        <v>40</v>
+      <c r="A14" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B6">
+  <conditionalFormatting sqref="B4">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>$B6=$B7</formula>
-    </cfRule>
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>$B6*0.95&lt;=$B7</formula>
+      <formula>Snapshot!$B$3="NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9:B14" type="list">
-      <formula1>OFFSET(States!$A$7,0,0,States!$B$4)</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6" type="whole">
+  <conditionalFormatting sqref="B11">
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>$B11=$B12</formula>
+    </cfRule>
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>$B11*0.95&lt;=$B12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="5">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B7 B9" type="list">
       <formula1>Misc!$B$1:$B$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4" type="none">
-      <formula1>Misc!$B$1:$B$2</formula1>
+    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A15:A18" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5:B6 B8" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B15:B18" type="list">
+      <formula1>INDEX(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2),SMALL(IF(ISTEXT(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2)),ROW(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2))-ROW(Attributes!$A$6),""),ROW(INDIRECT("1:"&amp;Attributes!$B$4))))</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2582,10 +3090,140 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.21"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="18"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <f aca="true">MATCH(1,INDEX(ISBLANK(OFFSET(B9,0,0,B6)),0,0),0)-1</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>$B6=$B7</formula>
+    </cfRule>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>$B6*0.95&lt;=$B7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9:B14" type="list">
+      <formula1>OFFSET(States!$A$7,0,0,States!$B$4)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="list">
+      <formula1>Misc!$B$1:$B$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4" type="none">
+      <formula1>Misc!$B$1:$B$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2602,94 +3240,94 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B1" s="18"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="B3" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="G6" s="4" t="n">
         <v>12</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="L6" s="4" t="n">
         <v>12</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="G7" s="4" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="L7" s="4" t="n">
         <v>6</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2701,7 +3339,7 @@
         <v>92</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -2713,7 +3351,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="K8" s="3" t="str">
         <f aca="false">IF(L10="YES","Min recruitment","ignored")</f>
@@ -2723,19 +3361,19 @@
         <v>35</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="str">
         <f aca="false">IF(B10="YES","Max recruitment",IF(B11="YES","ignored","Recruitment"))</f>
-        <v>ignored</v>
+        <v>Recruitment</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>50</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -2744,40 +3382,40 @@
         <v>Max recruitment</v>
       </c>
       <c r="G9" s="4" t="n">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="K9" s="3" t="str">
         <f aca="false">IF(L10="YES","Max recruitment",IF(L11="YES","ignored","Recruitment"))</f>
         <v>Recruitment</v>
       </c>
       <c r="L9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2786,41 +3424,41 @@
         <v>Random recruitment</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="F11" s="3" t="str">
         <f aca="false">IF(G10="YES","ignored","Random recruitment")</f>
         <v>ignored</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K11" s="3" t="str">
         <f aca="false">IF(L10="YES","ignored","Random recruitment")</f>
         <v>Random recruitment</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2832,7 +3470,7 @@
         <v>18.5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -2844,7 +3482,7 @@
         <v>18</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="K13" s="3" t="str">
         <f aca="false">IF(L12="YES","Recruitment age","ignored")</f>
@@ -2854,16 +3492,16 @@
         <v>18</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="str">
         <f aca="false">IF(AND(B10="NO",B11="YES"),"# of recruits distribution","ignored")</f>
-        <v># of recruits distribution</v>
+        <v>ignored</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2873,7 +3511,7 @@
         <v>ignored</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="H15" s="3"/>
       <c r="K15" s="3" t="str">
@@ -2881,14 +3519,14 @@
         <v>ignored</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="M15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="str">
         <f aca="false">IF(AND(B10="NO",B11="YES"),"# of distribution nodes","ignored")</f>
-        <v># of distribution nodes</v>
+        <v>ignored</v>
       </c>
       <c r="B16" s="21" t="n">
         <f aca="true">MATCH(1,ISBLANK(OFFSET(C18,0,0,1000)),0)-1</f>
@@ -2918,13 +3556,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="D17" s="0" t="str">
         <f aca="false">IF(B15="Pointwise","Normalised","")</f>
@@ -2935,13 +3573,13 @@
         <v>Total weight</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="I17" s="0" t="str">
         <f aca="false">IF(G15="Pointwise","Normalised","")</f>
@@ -2952,13 +3590,13 @@
         <v/>
       </c>
       <c r="K17" s="3" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="N17" s="0" t="str">
         <f aca="false">IF(L15="Pointwise","Normalised","")</f>
@@ -2971,7 +3609,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="n">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>25</v>
@@ -3015,7 +3653,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>20</v>
@@ -3059,7 +3697,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="n">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>30</v>
@@ -3103,7 +3741,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="n">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>25</v>
@@ -3181,7 +3819,7 @@
         <v>Recruitment age distribution</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="C23" s="3"/>
     </row>
@@ -3202,7 +3840,7 @@
         <v>Recruitment age distribution</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="H24" s="3"/>
       <c r="K24" s="3" t="str">
@@ -3210,19 +3848,19 @@
         <v>Recruitment age distribution</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="M24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(B23="Pointwise","Normalised","")</f>
@@ -3267,13 +3905,13 @@
         <v/>
       </c>
       <c r="F26" s="3" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="I26" s="0" t="str">
         <f aca="false">IF(G24="Pointwise","Normalised","")</f>
@@ -3284,13 +3922,13 @@
         <v/>
       </c>
       <c r="K26" s="3" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="N26" s="0" t="str">
         <f aca="false">IF(L24="Pointwise","Normalised","")</f>
@@ -3560,10 +4198,6 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7 G7 L7" type="decimal">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -3585,6 +4219,10 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B16 G16 L16 B24 G25 L25" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3600,7 +4238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3619,63 +4257,63 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="B1" s="18"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>45</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>67</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3697,234 +4335,6 @@
     </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7" type="list">
       <formula1>"EITHER,BOTH"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E16"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E12" activeCellId="0" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="18"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="0" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="D3" s="3" t="n">
-        <f aca="false">MATCH(1,INDEX(ISBLANK(D6:$AMJ6),0,0),0)-1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="E6" s="4" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:B3"/>
-  </mergeCells>
-  <dataValidations count="4">
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 D6:E6" type="decimal">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B12 D12:E12" type="list">
-      <formula1>INDEX(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2),SMALL(IF(ISTEXT(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2)),ROW(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2))-ROW(Attributes!$A$6),""),ROW(INDIRECT("1:"&amp;Attributes!$B$4))))</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5 B7:B10 D7:E10 B13:B16 D13:E16" type="list">
-      <formula1>Misc!$B$1:$B$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:E5" type="list">
-      <formula1>OFFSET(States!$A$7,0,0,States!$B$4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -3943,107 +4353,269 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="20.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="n">
-        <f aca="true">INDIRECT(CONCATENATE("'",General!B3,".xlsx'#$General.B2"))</f>
-        <v>0</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="str">
-        <f aca="false">IF(ISERR(A1),CONCATENATE("'[",General!B3,".xlsx]"),CONCATENATE("'",General!B3,".xlsx'#'"))</f>
-        <v>'simCatalogue.xlsx'#'</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="3" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="23"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="B4" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <f aca="true">MATCH(1,INDEX(ISBLANK(OFFSET(E11,0,0,B7+1)),0,0),0)-1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="11" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="11" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="11" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="str">
-        <f aca="false">IF(ISERR(A1),"!",".")</f>
-        <v>.</v>
-      </c>
-      <c r="B3" s="0"/>
-      <c r="C3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <f aca="true">INDIRECT(CONCATENATE(A2,"General'",A3,"B1"))</f>
-        <v>0</v>
-      </c>
-      <c r="B4" s="0"/>
-      <c r="C4" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="str">
-        <f aca="false">CONCATENATE(A2,"General'",A3)</f>
-        <v>'simCatalogue.xlsx'#'General'.</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="str">
-        <f aca="false">CONCATENATE(A2,"Attributes'",A3)</f>
-        <v>'simCatalogue.xlsx'#'Attributes'.</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="str">
-        <f aca="false">CONCATENATE(A2,"States'",A3)</f>
-        <v>'simCatalogue.xlsx'#'States'.</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>'Output plots (trans)'!$B$4="NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>$B7=$B8</formula>
+    </cfRule>
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>$B7*0.95&lt;=$B8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:B15">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>'Output plots (trans)'!$A11="YES"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:D15">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>'Output plots (trans)'!$A11="NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:B20">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>'Output plots (trans)'!$A16="YES"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:D20">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>'Output plots (trans)'!$A16="NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3:B4" type="list">
+      <formula1>Misc!$B$1:$B$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C11:D20" type="list">
+      <formula1>OFFSET(States!$A$7,0,0,States!$B$4)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A11:A20" type="list">
+      <formula1>Misc!$B$1:$B$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>